<commit_message>
Train model to filter out answers
</commit_message>
<xml_diff>
--- a/Validation Metrics/data/Example forms.xlsx
+++ b/Validation Metrics/data/Example forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys.sharepoint.com/sites/Infoland-Text-to-Case/Gedeelde documenten/General/Documentation/Forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A23A7044-D769-4D05-8E69-70D7A42FC71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{20608FF4-6213-44FB-8050-84711A59EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="3720" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
   <si>
     <t>Full story</t>
   </si>
@@ -943,7 +943,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1004,10 +1004,10 @@
       <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
@@ -1033,10 +1033,10 @@
       <c r="E3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
@@ -1062,10 +1062,10 @@
       <c r="E4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
       <c r="H4" t="s">
@@ -1091,10 +1091,10 @@
       <c r="E5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" t="s">
         <v>49</v>
       </c>
       <c r="H5" t="s">
@@ -1120,10 +1120,10 @@
       <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" t="s">
         <v>53</v>
       </c>
       <c r="H6" t="s">
@@ -1149,10 +1149,10 @@
       <c r="E7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" t="s">
         <v>58</v>
       </c>
       <c r="H7" t="s">
@@ -1207,11 +1207,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.58333333333333337</v>
+      <c r="F9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H9" t="s">
         <v>54</v>
@@ -1440,6 +1440,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003695A1D697DE7647BC4C0E20313B1610" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a0a87bef77048b227ceede24ca25e04c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4f29d57b-08d4-4845-bc15-760501bed384" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="423aea61016ec2a4621d181025ca66f3" ns2:_="">
     <xsd:import namespace="4f29d57b-08d4-4845-bc15-760501bed384"/>
@@ -1571,29 +1586,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{062C2D03-396B-408B-914B-60AFBEF728B5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E197143-E82F-495B-919B-5612A799206D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E197143-E82F-495B-919B-5612A799206D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21065BA-C84E-4188-A0B2-5912BC7D3054}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21065BA-C84E-4188-A0B2-5912BC7D3054}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{062C2D03-396B-408B-914B-60AFBEF728B5}"/>
 </file>
</xml_diff>

<commit_message>
Train trust model on all data
</commit_message>
<xml_diff>
--- a/Validation Metrics/data/Example forms.xlsx
+++ b/Validation Metrics/data/Example forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys.sharepoint.com/sites/Infoland-Text-to-Case/Gedeelde documenten/General/Documentation/Forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20608FF4-6213-44FB-8050-84711A59EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80EE5036-52E7-4F35-9094-69EAE434E91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="3720" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lunch" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>Full story</t>
   </si>
@@ -257,6 +257,73 @@
   </si>
   <si>
     <t>no tomatoes</t>
+  </si>
+  <si>
+    <t>Hello, this is Sarah from the finance department. I'm looking to organize a team lunch at Vapiano's restaurant. We have 8 people attending, and we're looking to do this next Thursday, April 21st.
+We're hoping to start the lunch at around 1 PM and finish by 2 PM so that everyone can get back to work on time. We have a budget of $20 per person, including taxes and gratuity.
+We're interested in Vapiano's because of the delicious food options and the great reviews we've heard from colleagues. We're hoping to reserve a private area or a large table that can accommodate our group comfortably.
+We do have a couple of dietary restrictions in our group, including one member who is allergic to nuts, so we'd appreciate it if you could provide some options that cater to them.
+Please let us know if you're available on the 21st and if you can accommodate our request. We look forward to enjoying a delicious meal at Vapiano's.
+Here are my contact details in case you need to reach out to me for any further information or questions. Thank you!</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>$20 per person</t>
+  </si>
+  <si>
+    <t>Thursday, April 21st</t>
+  </si>
+  <si>
+    <t>1 PM</t>
+  </si>
+  <si>
+    <t>2 PM</t>
+  </si>
+  <si>
+    <t>Vapiano</t>
+  </si>
+  <si>
+    <t>allergic to nuts</t>
+  </si>
+  <si>
+    <t>Hello, this is Mark from the sales department. I'm looking to organize a team lunch. We have 15 people attending, and we're hoping to do this next Friday, April 22nd.
+We're looking for a sit-down meal and hoping to set a budget of $30 per person. We're hoping to start the lunch at around 12:30 PM and finish by 2 PM.
+We also have a few dietary restrictions in our group, including a vegetarian and a member who is allergic to shellfish, so we'd appreciate it if the lunch can provide some options that can cater to them.</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>$30 per person</t>
+  </si>
+  <si>
+    <t>Friday, April 22nd</t>
+  </si>
+  <si>
+    <t>12:30 PM</t>
+  </si>
+  <si>
+    <t>a vegetarian and a member who is allergic to shellfish</t>
+  </si>
+  <si>
+    <t>Hello, my name is Lisa from the HR department. I'm looking to organize a team lunch. We have 10 people attending, and we're hoping to do this next Wednesday, April 20th.
+We're looking for a buffet-style lunch and hoping to set a budget of $25 per person. We're hoping to start the lunch at around 1 PM and finish by 2 PM.
+We also have a few dietary restrictions in our group, including a vegan and a member who is allergic to dairy, so we'd like if there are some options that can cater to them.
+Thank you, and have a great day!</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>$25 per person</t>
+  </si>
+  <si>
+    <t>Wednesday, April 20th</t>
+  </si>
+  <si>
+    <t>a vegan and a member who is allergic to dairy</t>
   </si>
   <si>
     <t>Is the incident reported by a third party?</t>
@@ -356,13 +423,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -396,9 +463,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,13 +1010,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4568475-A99B-451C-957E-B70D7460D3D6}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="66.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.140625" customWidth="1"/>
@@ -959,7 +1029,7 @@
     <col min="9" max="9" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1087,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.45">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1046,7 +1116,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1075,7 +1145,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.45">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1104,7 +1174,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -1133,7 +1203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1249,8 +1319,96 @@
         <v>73</v>
       </c>
     </row>
+    <row r="11" spans="1:9" ht="304.5">
+      <c r="A11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="130.5">
+      <c r="A12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="130.5">
+      <c r="A13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1258,13 +1416,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42EB2CD-C0EF-491D-B4DB-3B2C06DD9B46}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="202.7109375" customWidth="1"/>
+    <col min="1" max="1" width="161.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
@@ -1278,30 +1436,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1310,30 +1468,30 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1344,19 +1502,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D4" s="3">
         <v>0.33333333333333331</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -1367,71 +1525,71 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D7" s="3">
         <v>0.375</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1440,18 +1598,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1587,11 +1745,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E197143-E82F-495B-919B-5612A799206D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21065BA-C84E-4188-A0B2-5912BC7D3054}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A21065BA-C84E-4188-A0B2-5912BC7D3054}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E197143-E82F-495B-919B-5612A799206D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>